<commit_message>
Updated Luxury_Goods.xlsx with new data
</commit_message>
<xml_diff>
--- a/NAV/Luxury_Goods.xlsx
+++ b/NAV/Luxury_Goods.xlsx
@@ -506,7 +506,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J610"/>
+  <dimension ref="A1:J631"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A566" workbookViewId="0">
       <selection activeCell="G585" sqref="G585"/>
@@ -18572,6 +18572,657 @@
         <v>217.5326560482892</v>
       </c>
     </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>2024-08-28</t>
+        </is>
+      </c>
+      <c r="C611" t="n">
+        <v>1746.650024414062</v>
+      </c>
+      <c r="D611" t="n">
+        <v>1322.349975585938</v>
+      </c>
+      <c r="E611" t="n">
+        <v>1771.75</v>
+      </c>
+      <c r="F611" t="n">
+        <v>2073.949951171875</v>
+      </c>
+      <c r="G611" t="n">
+        <v>462.7999877929688</v>
+      </c>
+      <c r="H611" t="n">
+        <v>8303.099914550781</v>
+      </c>
+      <c r="I611" t="n">
+        <v>0</v>
+      </c>
+      <c r="J611" t="n">
+        <v>217.5326560482892</v>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>2024-08-29</t>
+        </is>
+      </c>
+      <c r="C612" t="n">
+        <v>1695.900024414062</v>
+      </c>
+      <c r="D612" t="n">
+        <v>1307.849975585938</v>
+      </c>
+      <c r="E612" t="n">
+        <v>1788.400024414062</v>
+      </c>
+      <c r="F612" t="n">
+        <v>2194.800048828125</v>
+      </c>
+      <c r="G612" t="n">
+        <v>465</v>
+      </c>
+      <c r="H612" t="n">
+        <v>8381.950073242188</v>
+      </c>
+      <c r="I612" t="n">
+        <v>0.009496472342001468</v>
+      </c>
+      <c r="J612" t="n">
+        <v>219.5984488999339</v>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>2024-08-30</t>
+        </is>
+      </c>
+      <c r="C613" t="n">
+        <v>1703.900024414062</v>
+      </c>
+      <c r="D613" t="n">
+        <v>1306.050048828125</v>
+      </c>
+      <c r="E613" t="n">
+        <v>1743.650024414062</v>
+      </c>
+      <c r="F613" t="n">
+        <v>2183.5</v>
+      </c>
+      <c r="G613" t="n">
+        <v>477.0499877929688</v>
+      </c>
+      <c r="H613" t="n">
+        <v>8368.250061035156</v>
+      </c>
+      <c r="I613" t="n">
+        <v>-0.001634465975974491</v>
+      </c>
+      <c r="J613" t="n">
+        <v>219.2395227068302</v>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>2024-09-02</t>
+        </is>
+      </c>
+      <c r="C614" t="n">
+        <v>1660.599975585938</v>
+      </c>
+      <c r="D614" t="n">
+        <v>1280.449951171875</v>
+      </c>
+      <c r="E614" t="n">
+        <v>1769.650024414062</v>
+      </c>
+      <c r="F614" t="n">
+        <v>2220.5</v>
+      </c>
+      <c r="G614" t="n">
+        <v>464.8500061035156</v>
+      </c>
+      <c r="H614" t="n">
+        <v>8325.749969482422</v>
+      </c>
+      <c r="I614" t="n">
+        <v>-0.005078731065963999</v>
+      </c>
+      <c r="J614" t="n">
+        <v>218.1260641319719</v>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>2024-09-03</t>
+        </is>
+      </c>
+      <c r="C615" t="n">
+        <v>1683.75</v>
+      </c>
+      <c r="D615" t="n">
+        <v>1248.449951171875</v>
+      </c>
+      <c r="E615" t="n">
+        <v>1810.949951171875</v>
+      </c>
+      <c r="F615" t="n">
+        <v>2205.5</v>
+      </c>
+      <c r="G615" t="n">
+        <v>469.6000061035156</v>
+      </c>
+      <c r="H615" t="n">
+        <v>8357.449920654297</v>
+      </c>
+      <c r="I615" t="n">
+        <v>0.003807458942205738</v>
+      </c>
+      <c r="J615" t="n">
+        <v>218.9565701653793</v>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>2024-09-04</t>
+        </is>
+      </c>
+      <c r="C616" t="n">
+        <v>1699.5</v>
+      </c>
+      <c r="D616" t="n">
+        <v>1288.900024414062</v>
+      </c>
+      <c r="E616" t="n">
+        <v>1780.25</v>
+      </c>
+      <c r="F616" t="n">
+        <v>2217.949951171875</v>
+      </c>
+      <c r="G616" t="n">
+        <v>466.5499877929688</v>
+      </c>
+      <c r="H616" t="n">
+        <v>8386.249938964844</v>
+      </c>
+      <c r="I616" t="n">
+        <v>0.003446029420932761</v>
+      </c>
+      <c r="J616" t="n">
+        <v>219.7111009480757</v>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>2024-09-05</t>
+        </is>
+      </c>
+      <c r="C617" t="n">
+        <v>1694.699951171875</v>
+      </c>
+      <c r="D617" t="n">
+        <v>1272.300048828125</v>
+      </c>
+      <c r="E617" t="n">
+        <v>1783.150024414062</v>
+      </c>
+      <c r="F617" t="n">
+        <v>2236.14990234375</v>
+      </c>
+      <c r="G617" t="n">
+        <v>467.75</v>
+      </c>
+      <c r="H617" t="n">
+        <v>8389.549926757812</v>
+      </c>
+      <c r="I617" t="n">
+        <v>0.0003934998142180441</v>
+      </c>
+      <c r="J617" t="n">
+        <v>219.7975572254804</v>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>2024-09-06</t>
+        </is>
+      </c>
+      <c r="C618" t="n">
+        <v>1724.449951171875</v>
+      </c>
+      <c r="D618" t="n">
+        <v>1234.300048828125</v>
+      </c>
+      <c r="E618" t="n">
+        <v>1778.650024414062</v>
+      </c>
+      <c r="F618" t="n">
+        <v>2224.39990234375</v>
+      </c>
+      <c r="G618" t="n">
+        <v>463.3999938964844</v>
+      </c>
+      <c r="H618" t="n">
+        <v>8351.999908447266</v>
+      </c>
+      <c r="I618" t="n">
+        <v>-0.004475808432915339</v>
+      </c>
+      <c r="J618" t="n">
+        <v>218.8137854653164</v>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>2024-09-09</t>
+        </is>
+      </c>
+      <c r="C619" t="n">
+        <v>1789.300048828125</v>
+      </c>
+      <c r="D619" t="n">
+        <v>1234.300048828125</v>
+      </c>
+      <c r="E619" t="n">
+        <v>1817.949951171875</v>
+      </c>
+      <c r="F619" t="n">
+        <v>2138.60009765625</v>
+      </c>
+      <c r="G619" t="n">
+        <v>460.7999877929688</v>
+      </c>
+      <c r="H619" t="n">
+        <v>8362.550109863281</v>
+      </c>
+      <c r="I619" t="n">
+        <v>0.001263194627833399</v>
+      </c>
+      <c r="J619" t="n">
+        <v>219.0901898636121</v>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>2024-09-10</t>
+        </is>
+      </c>
+      <c r="C620" t="n">
+        <v>1799.949951171875</v>
+      </c>
+      <c r="D620" t="n">
+        <v>1249.650024414062</v>
+      </c>
+      <c r="E620" t="n">
+        <v>1830.099975585938</v>
+      </c>
+      <c r="F620" t="n">
+        <v>2140.14990234375</v>
+      </c>
+      <c r="G620" t="n">
+        <v>466.9500122070312</v>
+      </c>
+      <c r="H620" t="n">
+        <v>8420.699890136719</v>
+      </c>
+      <c r="I620" t="n">
+        <v>0.006953594239734628</v>
+      </c>
+      <c r="J620" t="n">
+        <v>220.6136541458301</v>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>2024-09-11</t>
+        </is>
+      </c>
+      <c r="C621" t="n">
+        <v>1788.25</v>
+      </c>
+      <c r="D621" t="n">
+        <v>1255</v>
+      </c>
+      <c r="E621" t="n">
+        <v>1828.699951171875</v>
+      </c>
+      <c r="F621" t="n">
+        <v>2119.85009765625</v>
+      </c>
+      <c r="G621" t="n">
+        <v>459.2999877929688</v>
+      </c>
+      <c r="H621" t="n">
+        <v>8369.700012207031</v>
+      </c>
+      <c r="I621" t="n">
+        <v>-0.006056489198650145</v>
+      </c>
+      <c r="J621" t="n">
+        <v>219.2775099324211</v>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>2024-09-12</t>
+        </is>
+      </c>
+      <c r="C622" t="n">
+        <v>1816.650024414062</v>
+      </c>
+      <c r="D622" t="n">
+        <v>1257.449951171875</v>
+      </c>
+      <c r="E622" t="n">
+        <v>1852.949951171875</v>
+      </c>
+      <c r="F622" t="n">
+        <v>2111</v>
+      </c>
+      <c r="G622" t="n">
+        <v>459</v>
+      </c>
+      <c r="H622" t="n">
+        <v>8415.049926757812</v>
+      </c>
+      <c r="I622" t="n">
+        <v>0.005418344084571652</v>
+      </c>
+      <c r="J622" t="n">
+        <v>220.4656309312431</v>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>2024-09-13</t>
+        </is>
+      </c>
+      <c r="C623" t="n">
+        <v>1888</v>
+      </c>
+      <c r="D623" t="n">
+        <v>1264.349975585938</v>
+      </c>
+      <c r="E623" t="n">
+        <v>1921.550048828125</v>
+      </c>
+      <c r="F623" t="n">
+        <v>2101.35009765625</v>
+      </c>
+      <c r="G623" t="n">
+        <v>451.75</v>
+      </c>
+      <c r="H623" t="n">
+        <v>8530.500122070312</v>
+      </c>
+      <c r="I623" t="n">
+        <v>0.01371949023681921</v>
+      </c>
+      <c r="J623" t="n">
+        <v>223.4903070023585</v>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>2024-09-16</t>
+        </is>
+      </c>
+      <c r="C624" t="n">
+        <v>1934.900024414062</v>
+      </c>
+      <c r="D624" t="n">
+        <v>1259.75</v>
+      </c>
+      <c r="E624" t="n">
+        <v>1916</v>
+      </c>
+      <c r="F624" t="n">
+        <v>2047.199951171875</v>
+      </c>
+      <c r="G624" t="n">
+        <v>447.8999938964844</v>
+      </c>
+      <c r="H624" t="n">
+        <v>8501.549957275391</v>
+      </c>
+      <c r="I624" t="n">
+        <v>-0.003393724210849177</v>
+      </c>
+      <c r="J624" t="n">
+        <v>222.7318425365945</v>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>2024-09-17</t>
+        </is>
+      </c>
+      <c r="C625" t="n">
+        <v>1891.199951171875</v>
+      </c>
+      <c r="D625" t="n">
+        <v>1257.550048828125</v>
+      </c>
+      <c r="E625" t="n">
+        <v>1904.050048828125</v>
+      </c>
+      <c r="F625" t="n">
+        <v>2034.699951171875</v>
+      </c>
+      <c r="G625" t="n">
+        <v>452.75</v>
+      </c>
+      <c r="H625" t="n">
+        <v>8445.75</v>
+      </c>
+      <c r="I625" t="n">
+        <v>-0.006563504014657771</v>
+      </c>
+      <c r="J625" t="n">
+        <v>221.2699411939134</v>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>2024-09-18</t>
+        </is>
+      </c>
+      <c r="C626" t="n">
+        <v>1879.449951171875</v>
+      </c>
+      <c r="D626" t="n">
+        <v>1232.050048828125</v>
+      </c>
+      <c r="E626" t="n">
+        <v>1889.400024414062</v>
+      </c>
+      <c r="F626" t="n">
+        <v>2042.550048828125</v>
+      </c>
+      <c r="G626" t="n">
+        <v>448.8500061035156</v>
+      </c>
+      <c r="H626" t="n">
+        <v>8390.000091552734</v>
+      </c>
+      <c r="I626" t="n">
+        <v>-0.006600942302017657</v>
+      </c>
+      <c r="J626" t="n">
+        <v>219.8093510789215</v>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>2024-09-19</t>
+        </is>
+      </c>
+      <c r="C627" t="n">
+        <v>1866.650024414062</v>
+      </c>
+      <c r="D627" t="n">
+        <v>1234.5</v>
+      </c>
+      <c r="E627" t="n">
+        <v>1929.199951171875</v>
+      </c>
+      <c r="F627" t="n">
+        <v>2025.699951171875</v>
+      </c>
+      <c r="G627" t="n">
+        <v>450</v>
+      </c>
+      <c r="H627" t="n">
+        <v>8406.049926757812</v>
+      </c>
+      <c r="I627" t="n">
+        <v>0.00191297199403341</v>
+      </c>
+      <c r="J627" t="n">
+        <v>220.2298402115621</v>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>2024-09-20</t>
+        </is>
+      </c>
+      <c r="C628" t="n">
+        <v>1930.099975585938</v>
+      </c>
+      <c r="D628" t="n">
+        <v>1246.550048828125</v>
+      </c>
+      <c r="E628" t="n">
+        <v>1928.400024414062</v>
+      </c>
+      <c r="F628" t="n">
+        <v>2062.300048828125</v>
+      </c>
+      <c r="G628" t="n">
+        <v>446.7999877929688</v>
+      </c>
+      <c r="H628" t="n">
+        <v>8507.750061035156</v>
+      </c>
+      <c r="I628" t="n">
+        <v>0.01209844518691423</v>
+      </c>
+      <c r="J628" t="n">
+        <v>222.8942788618846</v>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>2024-09-23</t>
+        </is>
+      </c>
+      <c r="C629" t="n">
+        <v>2012.849975585938</v>
+      </c>
+      <c r="D629" t="n">
+        <v>1229.900024414062</v>
+      </c>
+      <c r="E629" t="n">
+        <v>1882.449951171875</v>
+      </c>
+      <c r="F629" t="n">
+        <v>2039</v>
+      </c>
+      <c r="G629" t="n">
+        <v>445.75</v>
+      </c>
+      <c r="H629" t="n">
+        <v>8501.449951171875</v>
+      </c>
+      <c r="I629" t="n">
+        <v>-0.000740514215636784</v>
+      </c>
+      <c r="J629" t="n">
+        <v>222.7292224798032</v>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>2024-09-24</t>
+        </is>
+      </c>
+      <c r="C630" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D630" t="n">
+        <v>1238.800048828125</v>
+      </c>
+      <c r="E630" t="n">
+        <v>1914.400024414062</v>
+      </c>
+      <c r="F630" t="n">
+        <v>2064.550048828125</v>
+      </c>
+      <c r="G630" t="n">
+        <v>439.25</v>
+      </c>
+      <c r="H630" t="n">
+        <v>8561.500122070312</v>
+      </c>
+      <c r="I630" t="n">
+        <v>0.007063521075032611</v>
+      </c>
+      <c r="J630" t="n">
+        <v>224.302475036815</v>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>2024-09-25</t>
+        </is>
+      </c>
+      <c r="C631" t="n">
+        <v>2051.39990234375</v>
+      </c>
+      <c r="D631" t="n">
+        <v>1252.949951171875</v>
+      </c>
+      <c r="E631" t="n">
+        <v>1910.849975585938</v>
+      </c>
+      <c r="F631" t="n">
+        <v>2112.050048828125</v>
+      </c>
+      <c r="G631" t="n">
+        <v>441.5499877929688</v>
+      </c>
+      <c r="H631" t="n">
+        <v>8651.899841308594</v>
+      </c>
+      <c r="I631" t="n">
+        <v>0.01055886444540762</v>
+      </c>
+      <c r="J631" t="n">
+        <v>226.6708544654981</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>